<commit_message>
Working Birthday announcer, birthday field in BirthdayUser.java not assigning correctly though.
</commit_message>
<xml_diff>
--- a/src/main/resources/birthdays.xlsx
+++ b/src/main/resources/birthdays.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Proba\IdeaProjects\Jinseo_Bot\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB6C8E7F-B573-4C64-9616-4671146437E8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9148A32-BC02-4C00-926D-55B2B88608C0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{3A43137D-FF13-441C-8D27-8175FD9C3C57}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
     <t>Jack</t>
   </si>
@@ -112,15 +112,42 @@
   </si>
   <si>
     <t>"367346612441448458"</t>
+  </si>
+  <si>
+    <t>06/11/2020</t>
+  </si>
+  <si>
+    <t>05/13/2020</t>
+  </si>
+  <si>
+    <t>08/17/2020</t>
+  </si>
+  <si>
+    <t>07/29/2020</t>
+  </si>
+  <si>
+    <t>05/27/2020</t>
+  </si>
+  <si>
+    <t>04/05/2020</t>
+  </si>
+  <si>
+    <t>07/03/2020</t>
+  </si>
+  <si>
+    <t>12/22/2020</t>
+  </si>
+  <si>
+    <t>11/06/2020</t>
+  </si>
+  <si>
+    <t>10/14/2020</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
-  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -155,7 +182,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -473,7 +500,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C12"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -503,8 +530,8 @@
       <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2">
-        <v>43993</v>
+      <c r="C2" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="D2" t="s">
         <v>17</v>
@@ -517,8 +544,8 @@
       <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2">
-        <v>43964</v>
+      <c r="C3" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="D3" t="s">
         <v>18</v>
@@ -531,8 +558,8 @@
       <c r="B4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="2">
-        <v>44060</v>
+      <c r="C4" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="D4" t="s">
         <v>19</v>
@@ -545,8 +572,8 @@
       <c r="B5" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="2">
-        <v>44041</v>
+      <c r="C5" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="D5" t="s">
         <v>20</v>
@@ -559,8 +586,8 @@
       <c r="B6" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="2">
-        <v>44178</v>
+      <c r="C6" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="D6" t="s">
         <v>15</v>
@@ -573,8 +600,8 @@
       <c r="B7" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="2">
-        <v>43978</v>
+      <c r="C7" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="D7" t="s">
         <v>16</v>
@@ -587,8 +614,8 @@
       <c r="B8" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="2">
-        <v>43926</v>
+      <c r="C8" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="D8" t="s">
         <v>21</v>
@@ -601,8 +628,8 @@
       <c r="B9" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="2">
-        <v>44015</v>
+      <c r="C9" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="D9" t="s">
         <v>22</v>
@@ -615,8 +642,8 @@
       <c r="B10" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="2">
-        <v>44187</v>
+      <c r="C10" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="D10" t="s">
         <v>25</v>
@@ -629,8 +656,8 @@
       <c r="B11" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="2">
-        <v>44141</v>
+      <c r="C11" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="D11" t="s">
         <v>23</v>
@@ -643,8 +670,8 @@
       <c r="B12" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="2">
-        <v>44118</v>
+      <c r="C12" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="D12" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
Top posts and controversial posts are working
</commit_message>
<xml_diff>
--- a/src/main/resources/birthdays.xlsx
+++ b/src/main/resources/birthdays.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Proba\IdeaProjects\Jinseo_Bot\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9148A32-BC02-4C00-926D-55B2B88608C0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92258AD6-B9B1-4115-8417-E5AA9417B43A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{3A43137D-FF13-441C-8D27-8175FD9C3C57}"/>
   </bookViews>
@@ -135,13 +135,13 @@
     <t>07/03/2020</t>
   </si>
   <si>
-    <t>12/22/2020</t>
-  </si>
-  <si>
     <t>11/06/2020</t>
   </si>
   <si>
     <t>10/14/2020</t>
+  </si>
+  <si>
+    <t>12/21/2020</t>
   </si>
 </sst>
 </file>
@@ -500,7 +500,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -643,7 +643,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D10" t="s">
         <v>25</v>
@@ -657,7 +657,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D11" t="s">
         <v>23</v>
@@ -671,7 +671,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D12" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
Added automatic weekly and daily timer tasks for Birthday and message reactions
</commit_message>
<xml_diff>
--- a/src/main/resources/birthdays.xlsx
+++ b/src/main/resources/birthdays.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Proba\IdeaProjects\Jinseo_Bot\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92258AD6-B9B1-4115-8417-E5AA9417B43A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0250A4E3-0153-43BF-89CE-E6D7AE17B031}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{3A43137D-FF13-441C-8D27-8175FD9C3C57}"/>
   </bookViews>
@@ -141,7 +141,7 @@
     <t>10/14/2020</t>
   </si>
   <si>
-    <t>12/21/2020</t>
+    <t>12/22/2020</t>
   </si>
 </sst>
 </file>
@@ -500,7 +500,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>